<commit_message>
Complementos guiones 03 y 12 de octavo CS
Ajustes a imagenes y pies en CE CS_08_03 despues de legalizacion y
nuevas asiganciones de recursos CS_08_12
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion12/CS_08_12_CO_Escaleta.xlsx
+++ b/fuentes/contenidos/grado08/guion12/CS_08_12_CO_Escaleta.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="219">
   <si>
     <t>Asignatura</t>
   </si>
@@ -676,6 +676,12 @@
   </si>
   <si>
     <t>Asignado a Ana Hoyos (11/03/16)</t>
+  </si>
+  <si>
+    <t>Asignado a Ana Hoyos (14/03/16)</t>
+  </si>
+  <si>
+    <t>Asignado a Diego Espitia (14/03/16)</t>
   </si>
 </sst>
 </file>
@@ -962,6 +968,24 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -981,24 +1005,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1309,7 +1315,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,94 +1344,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="57" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="58" t="s">
+      <c r="M1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="58"/>
-      <c r="O1" s="55" t="s">
+      <c r="N1" s="51"/>
+      <c r="O1" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="55" t="s">
+      <c r="P1" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="Q1" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="56" t="s">
+      <c r="S1" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="57" t="s">
+      <c r="T1" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="56" t="s">
+      <c r="U1" s="49" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="51"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="57"/>
       <c r="D2" s="38"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="48"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="54"/>
       <c r="M2" s="39" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="56"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="49"/>
     </row>
     <row r="3" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -1619,7 +1625,9 @@
       <c r="N6" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="O6" s="12"/>
+      <c r="O6" s="12" t="s">
+        <v>217</v>
+      </c>
       <c r="P6" s="12" t="s">
         <v>19</v>
       </c>
@@ -2238,10 +2246,10 @@
       <c r="D17" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="F17" s="54" t="s">
+      <c r="F17" s="47" t="s">
         <v>167</v>
       </c>
       <c r="G17" s="22" t="s">
@@ -2299,8 +2307,8 @@
       <c r="D18" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="E18" s="53"/>
-      <c r="F18" s="54"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="47"/>
       <c r="G18" s="22" t="s">
         <v>169</v>
       </c>
@@ -2385,7 +2393,9 @@
       <c r="N19" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="O19" s="12"/>
+      <c r="O19" s="12" t="s">
+        <v>217</v>
+      </c>
       <c r="P19" s="12" t="s">
         <v>19</v>
       </c>
@@ -2598,7 +2608,9 @@
       <c r="N23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="O23" s="12"/>
+      <c r="O23" s="12" t="s">
+        <v>218</v>
+      </c>
       <c r="P23" s="12" t="s">
         <v>19</v>
       </c>
@@ -3795,16 +3807,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="M1:N1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="L1:L2"/>
@@ -3816,6 +3818,16 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>